<commit_message>
benchmarking against other libraries
</commit_message>
<xml_diff>
--- a/dev/perf_stats.xlsx
+++ b/dev/perf_stats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\unity\mgGif\dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99A3C5E3-AF22-4EC8-AE9C-28B1A34D3043}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{838ABC14-4C7A-45EB-B889-EDE20D07CF5B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{5250E78F-E47C-4383-8E14-7124FB922824}"/>
+    <workbookView xWindow="38290" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{5250E78F-E47C-4383-8E14-7124FB922824}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="11">
   <si>
     <t>Laptop</t>
   </si>
@@ -61,6 +61,12 @@
   </si>
   <si>
     <t>% Diff</t>
+  </si>
+  <si>
+    <t>UniGif</t>
+  </si>
+  <si>
+    <t>Unity-GifDecoder</t>
   </si>
 </sst>
 </file>
@@ -219,9 +225,23 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="3" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="8" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="5" xfId="2" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -230,20 +250,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="3" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="3" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="3" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="8" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="3" fillId="3" borderId="5" xfId="2" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="20% - Accent3" xfId="3" builtinId="38"/>
@@ -561,157 +568,214 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A88638F9-5EA6-440E-8015-2A5E504DACB8}">
-  <dimension ref="B1:K6"/>
+  <dimension ref="B1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="2.7265625" customWidth="1"/>
-    <col min="2" max="2" width="13.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="10" width="14.08984375" customWidth="1"/>
+    <col min="2" max="2" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="11" width="11.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="2" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B2" s="1"/>
-      <c r="C2" s="1" t="s">
+      <c r="B2" s="12"/>
+      <c r="C2" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="1" t="s">
+      <c r="D2" s="14"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="2"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="2" t="s">
+      <c r="G2" s="14"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="2"/>
-      <c r="K2" s="3"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="15"/>
     </row>
     <row r="3" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B3" s="12"/>
-      <c r="C3" s="6" t="s">
+      <c r="B3" s="13"/>
+      <c r="C3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="G3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="9" t="s">
+      <c r="H3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="I3" s="8" t="s">
+      <c r="I3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="J3" s="8" t="s">
+      <c r="J3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="K3" s="9" t="s">
+      <c r="K3" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="2">
         <v>290</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="1">
         <v>315</v>
       </c>
-      <c r="E4" s="15">
+      <c r="E4" s="11">
         <f>1-D4/C4</f>
         <v>-8.6206896551724199E-2</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="2">
         <v>142</v>
       </c>
-      <c r="G4" s="4">
+      <c r="G4" s="1">
         <v>119</v>
       </c>
-      <c r="H4" s="13">
+      <c r="H4" s="9">
         <f>1-G4/F4</f>
         <v>0.1619718309859155</v>
       </c>
-      <c r="I4" s="4">
+      <c r="I4" s="1">
         <v>97</v>
       </c>
-      <c r="J4" s="4">
+      <c r="J4" s="1">
         <v>79</v>
       </c>
-      <c r="K4" s="13">
+      <c r="K4" s="9">
         <f>1-J4/I4</f>
         <v>0.18556701030927836</v>
       </c>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="2">
         <v>247</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="1">
         <v>280</v>
       </c>
-      <c r="E5" s="15">
+      <c r="E5" s="11">
         <f>1-D5/C5</f>
         <v>-0.1336032388663968</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="2">
         <v>112</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G5" s="1">
         <v>106</v>
       </c>
-      <c r="H5" s="13">
+      <c r="H5" s="9">
         <f>1-G5/F5</f>
         <v>5.3571428571428603E-2</v>
       </c>
-      <c r="I5" s="4">
+      <c r="I5" s="1">
         <v>80</v>
       </c>
-      <c r="J5" s="4">
+      <c r="J5" s="1">
         <v>70</v>
       </c>
-      <c r="K5" s="13">
+      <c r="K5" s="9">
         <f t="shared" ref="K5:K6" si="0">1-J5/I5</f>
         <v>0.125</v>
       </c>
     </row>
     <row r="6" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="10"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="8">
+      <c r="C6" s="7"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="5">
         <v>180</v>
       </c>
-      <c r="J6" s="8">
+      <c r="J6" s="5">
         <v>111</v>
       </c>
-      <c r="K6" s="14">
+      <c r="K6" s="10">
         <f t="shared" si="0"/>
         <v>0.3833333333333333</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10">
+        <v>7321</v>
+      </c>
+      <c r="E10" s="16">
+        <f>1-C$5/C10</f>
+        <v>0.96626143969403089</v>
+      </c>
+      <c r="F10">
+        <v>3790</v>
+      </c>
+      <c r="H10" s="16">
+        <f>1-F$5/F10</f>
+        <v>0.97044854881266496</v>
+      </c>
+      <c r="I10">
+        <v>3178</v>
+      </c>
+      <c r="K10" s="16">
+        <f>1-I$5/I10</f>
+        <v>0.97482693517935803</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11">
+        <v>365</v>
+      </c>
+      <c r="E11" s="16">
+        <f>1-C$5/C11</f>
+        <v>0.32328767123287672</v>
+      </c>
+      <c r="F11">
+        <v>123</v>
+      </c>
+      <c r="H11" s="16">
+        <f>1-F$5/F11</f>
+        <v>8.9430894308943132E-2</v>
+      </c>
+      <c r="I11">
+        <v>88</v>
+      </c>
+      <c r="K11" s="16">
+        <f>1-I$5/I11</f>
+        <v>9.0909090909090939E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>